<commit_message>
Make mcc172acquireDF more robust
</commit_message>
<xml_diff>
--- a/examples/PIconfig.xlsx
+++ b/examples/PIconfig.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakez\.julia\dev\MccDaqHats\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B64EC482-82D3-466E-8C0D-3E6B41DFCE46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45690D29-72F0-4DEF-88C1-DBE03B152E8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3465" yWindow="570" windowWidth="21600" windowHeight="14130" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3465" yWindow="570" windowWidth="21600" windowHeight="14130" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" r:id="rId1"/>
@@ -589,7 +589,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -680,12 +680,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
     <col min="8" max="8" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Remove nchan from Excel file
</commit_message>
<xml_diff>
--- a/examples/PIconfig.xlsx
+++ b/examples/PIconfig.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakez\.julia\dev\MccDaqHats\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EAC6FD8-45B4-4E2F-9CC0-13FBF9A2BAA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D77F49C1-D3A3-4E5D-B77D-BB077BA0B56F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3465" yWindow="570" windowWidth="21600" windowHeight="14130" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29295" yWindow="1350" windowWidth="21600" windowHeight="14130" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="40">
   <si>
     <t>Item</t>
   </si>
@@ -35,12 +35,6 @@
   </si>
   <si>
     <t>Comments</t>
-  </si>
-  <si>
-    <t>numchans</t>
-  </si>
-  <si>
-    <t>number of channels on chanconfig sheet, whether enabled or not</t>
   </si>
   <si>
     <t>time</t>
@@ -581,10 +575,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -605,63 +599,52 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>4</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <f>51200/1</f>
+        <v>51200</v>
+      </c>
+      <c r="D3" t="s">
         <v>5</v>
-      </c>
-      <c r="B3">
-        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="B4">
-        <f>51200/1</f>
-        <v>51200</v>
+        <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>34</v>
       </c>
-      <c r="B5">
-        <v>1</v>
+      <c r="B5" t="s">
+        <v>35</v>
       </c>
       <c r="D5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
         <v>39</v>
-      </c>
-      <c r="B7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D7" t="s">
-        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -686,31 +669,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>12</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>13</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>14</v>
-      </c>
-      <c r="H1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -722,16 +705,16 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
         <v>17</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>18</v>
-      </c>
-      <c r="E2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" t="s">
-        <v>20</v>
       </c>
       <c r="G2" t="b">
         <f>FALSE()</f>
@@ -741,7 +724,7 @@
         <v>1000</v>
       </c>
       <c r="I2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -753,16 +736,16 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" t="s">
         <v>22</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>23</v>
-      </c>
-      <c r="E3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" t="s">
-        <v>25</v>
       </c>
       <c r="G3" t="b">
         <f>TRUE()</f>
@@ -772,7 +755,7 @@
         <v>10</v>
       </c>
       <c r="I3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -784,16 +767,16 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G4" t="b">
         <f>TRUE()</f>
@@ -803,7 +786,7 @@
         <v>10</v>
       </c>
       <c r="I4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -815,16 +798,16 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G5" t="b">
         <f>TRUE()</f>
@@ -834,39 +817,39 @@
         <v>10</v>
       </c>
       <c r="I5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C10" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C11" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C12" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D12" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C13" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>